<commit_message>
Presentacion5 parte de estimacion de costes acabada.
Se amplia el excel.
</commit_message>
<xml_diff>
--- a/Documentos_generados/5. Costes y Justificación técnica/Estimacion costes.xlsx
+++ b/Documentos_generados/5. Costes y Justificación técnica/Estimacion costes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>Estimación costes</t>
   </si>
@@ -205,6 +205,96 @@
   </si>
   <si>
     <t>Costes Maateriales</t>
+  </si>
+  <si>
+    <t>Empleados</t>
+  </si>
+  <si>
+    <t>meses</t>
+  </si>
+  <si>
+    <t>dias/mes</t>
+  </si>
+  <si>
+    <t>Valoracion trabajo (€/h)</t>
+  </si>
+  <si>
+    <t>horas / dia</t>
+  </si>
+  <si>
+    <t>Se pacta este precio con la empresa desarrolladora de SW acorde a los datos de trabajadores</t>
+  </si>
+  <si>
+    <t>Almacen</t>
+  </si>
+  <si>
+    <t>Tecnico</t>
+  </si>
+  <si>
+    <t>Tecnicos</t>
+  </si>
+  <si>
+    <t>Vehiculos</t>
+  </si>
+  <si>
+    <t>Coste Vehiculos</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Instalacion</t>
+  </si>
+  <si>
+    <t>Salario</t>
+  </si>
+  <si>
+    <t>Coste/usuario</t>
+  </si>
+  <si>
+    <t>usuarios</t>
+  </si>
+  <si>
+    <t>Costes Contingencias</t>
+  </si>
+  <si>
+    <t>Materiales</t>
+  </si>
+  <si>
+    <t>RRHH</t>
+  </si>
+  <si>
+    <t>Subcontrataciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riesgo </t>
+  </si>
+  <si>
+    <t>% de guarda</t>
+  </si>
+  <si>
+    <t>Coste estimado</t>
+  </si>
+  <si>
+    <t>PRESUPUESTO</t>
+  </si>
+  <si>
+    <t>Recursos materiales</t>
+  </si>
+  <si>
+    <t>Recursos Humanos</t>
+  </si>
+  <si>
+    <t>Contingencias</t>
+  </si>
+  <si>
+    <t>Linea base de costes</t>
+  </si>
+  <si>
+    <t>Reservas de gestión</t>
+  </si>
+  <si>
+    <t>Presuesto total</t>
   </si>
 </sst>
 </file>
@@ -269,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +408,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -331,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -339,35 +471,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -375,13 +483,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -396,34 +498,131 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,20 +925,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T40"/>
+  <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="17"/>
+    <col min="2" max="2" width="13.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -750,47 +949,48 @@
     <col min="14" max="14" width="7.7109375" customWidth="1"/>
     <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="18" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" customWidth="1"/>
     <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" style="31" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="T1" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -798,35 +998,35 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="23">
         <v>2000</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
       <c r="R3">
         <v>12</v>
       </c>
       <c r="S3" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="31">
+      <c r="T3" s="19">
         <f>B3*R3</f>
         <v>24000</v>
       </c>
@@ -835,26 +1035,26 @@
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="23">
         <v>500</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="23"/>
+      <c r="E4" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="T4" s="31">
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="T4" s="19">
         <v>500</v>
       </c>
     </row>
@@ -862,35 +1062,35 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="23">
         <v>250</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
       <c r="R5">
         <v>20</v>
       </c>
       <c r="S5" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="19">
         <f>B5*R5</f>
         <v>5000</v>
       </c>
@@ -899,35 +1099,35 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="23">
         <v>700</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
       <c r="R6">
         <v>20</v>
       </c>
       <c r="S6" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="31">
+      <c r="T6" s="19">
         <f>B6*R6</f>
         <v>14000</v>
       </c>
@@ -936,92 +1136,92 @@
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="23">
         <v>150</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
       <c r="R7">
         <v>20</v>
       </c>
       <c r="S7" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="31">
+      <c r="T7" s="19">
         <f>B7*R7</f>
         <v>3000</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="23">
         <v>50</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
       <c r="R9">
         <v>160</v>
       </c>
       <c r="S9" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="31">
+      <c r="T9" s="19">
         <f>B9*R9</f>
         <v>8000</v>
       </c>
@@ -1030,35 +1230,35 @@
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="23">
         <v>20</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
       <c r="R10">
         <v>160</v>
       </c>
       <c r="S10" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="31">
+      <c r="T10" s="19">
         <f t="shared" ref="T10:T12" si="0">B10*R10</f>
         <v>3200</v>
       </c>
@@ -1067,35 +1267,35 @@
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="23">
         <v>37.5</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
       <c r="R11">
         <v>160</v>
       </c>
       <c r="S11" t="s">
         <v>17</v>
       </c>
-      <c r="T11" s="31">
+      <c r="T11" s="19">
         <f t="shared" si="0"/>
         <v>6000</v>
       </c>
@@ -1104,55 +1304,55 @@
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="24">
         <v>150</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
       <c r="R12" s="1">
         <v>160</v>
       </c>
-      <c r="S12" s="33" t="s">
+      <c r="S12" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="32">
+      <c r="T12" s="20">
         <f t="shared" si="0"/>
         <v>24000</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="T14" s="31">
+      <c r="T14" s="19">
         <f>SUM(T1:T12)</f>
         <v>87700</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1160,33 +1360,33 @@
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="9">
         <v>90000</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="9">
         <f>B17/1764</f>
         <v>51.020408163265309</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
       <c r="R17">
         <v>1</v>
       </c>
       <c r="S17" t="s">
         <v>18</v>
       </c>
-      <c r="T17" s="31">
+      <c r="T17" s="19">
         <f>B17*R17</f>
         <v>90000</v>
       </c>
@@ -1195,77 +1395,77 @@
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="9">
         <v>70000</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="9">
         <f>B18/1764</f>
         <v>39.682539682539684</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
       <c r="R18">
         <v>4</v>
       </c>
       <c r="S18" t="s">
         <v>18</v>
       </c>
-      <c r="T18" s="31">
+      <c r="T18" s="19">
         <f>B18*R18</f>
         <v>280000</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
     </row>
     <row r="20" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7" t="s">
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8" t="s">
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="9" t="s">
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
     </row>
     <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -1274,7 +1474,7 @@
       <c r="H21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -1283,7 +1483,7 @@
       <c r="K21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="M21" s="2" t="s">
@@ -1292,7 +1492,7 @@
       <c r="N21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O21" s="10" t="s">
+      <c r="O21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="P21" s="2" t="s">
@@ -1303,23 +1503,23 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="35">
+      <c r="B22" s="32">
         <v>56000</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="30">
         <f>B22/1764</f>
         <v>31.746031746031747</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="27" t="s">
         <v>50</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G22">
@@ -1329,7 +1529,7 @@
         <f>$B$22*G22/100</f>
         <v>56000</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="J22">
@@ -1339,7 +1539,7 @@
         <f>$B$22*J22/100</f>
         <v>56000</v>
       </c>
-      <c r="L22" s="11" t="s">
+      <c r="L22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="M22">
@@ -1349,7 +1549,7 @@
         <f>$B$22*M22/100</f>
         <v>56000</v>
       </c>
-      <c r="O22" s="11" t="s">
+      <c r="O22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="P22">
@@ -1361,14 +1561,14 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="27"/>
       <c r="E23" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G23">
@@ -1378,7 +1578,7 @@
         <f>B22*G23/100</f>
         <v>44800</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="J23">
@@ -1388,7 +1588,7 @@
         <f>$B$25*J23/100</f>
         <v>35800</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="L23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="M23">
@@ -1398,7 +1598,7 @@
         <f>$B$25*M23/100</f>
         <v>31325</v>
       </c>
-      <c r="O23" s="11" t="s">
+      <c r="O23" s="5" t="s">
         <v>33</v>
       </c>
       <c r="P23">
@@ -1410,14 +1610,14 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="27"/>
       <c r="E24" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="G24">
@@ -1427,7 +1627,7 @@
         <f>$B$25*G24/100</f>
         <v>31325</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="J24">
@@ -1437,7 +1637,7 @@
         <f>$B$25*J24/100</f>
         <v>22375</v>
       </c>
-      <c r="L24" s="14" t="s">
+      <c r="L24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="M24">
@@ -1447,7 +1647,7 @@
         <f>$B$25*M24/100</f>
         <v>22375</v>
       </c>
-      <c r="O24" s="14" t="s">
+      <c r="O24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="P24">
@@ -1459,23 +1659,23 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="32">
         <v>44750</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="30">
         <f t="shared" ref="C25" si="1">B25/1764</f>
         <v>25.368480725623584</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="27" t="s">
         <v>50</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G25">
@@ -1485,7 +1685,7 @@
         <f>$B$28*G25/100</f>
         <v>18720</v>
       </c>
-      <c r="O25" s="15" t="s">
+      <c r="O25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="P25">
@@ -1497,14 +1697,14 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="27"/>
       <c r="E26" t="s">
         <v>29</v>
       </c>
-      <c r="O26" s="15" t="s">
+      <c r="O26" s="7" t="s">
         <v>35</v>
       </c>
       <c r="P26">
@@ -1516,176 +1716,511 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="18" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="18"/>
+      <c r="G27" s="29"/>
       <c r="H27">
         <f>SUM(H22:H26)</f>
         <v>150845</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="18"/>
+      <c r="J27" s="29"/>
       <c r="K27">
         <f>SUM(K22:K26)</f>
         <v>114175</v>
       </c>
-      <c r="L27" s="18" t="s">
+      <c r="L27" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="M27" s="18"/>
+      <c r="M27" s="29"/>
       <c r="N27">
         <f>SUM(N22:N26)</f>
         <v>109700</v>
       </c>
-      <c r="O27" s="18" t="s">
+      <c r="O27" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="P27" s="18"/>
+      <c r="P27" s="29"/>
       <c r="Q27">
         <f>SUM(Q22:Q26)</f>
         <v>188360</v>
       </c>
-      <c r="T27" s="31">
+      <c r="T27" s="19">
         <f>SUM(H27,K27,N27,Q27)</f>
         <v>563080</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="35">
+      <c r="B28" s="32">
         <v>31200</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="30">
         <f t="shared" ref="C28" si="2">B28/1764</f>
         <v>17.687074829931973</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="27" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="3"/>
-      <c r="T29" s="31">
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="27"/>
+      <c r="T29" s="19">
         <f>SUM(T15:T28)</f>
         <v>933080</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+    <row r="33" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="B33" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="17">
-        <v>200000</v>
-      </c>
-      <c r="T34" s="31">
-        <f>B34</f>
-        <v>200000</v>
+      <c r="B34" s="9">
+        <v>10</v>
+      </c>
+      <c r="C34" s="38">
+        <v>50</v>
+      </c>
+      <c r="D34" s="1">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <v>20</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="T34" s="19">
+        <f>B34*C34*D34*E34*F34</f>
+        <v>320000</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="43"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="17">
-        <v>120000</v>
-      </c>
-      <c r="T35" s="31">
-        <f>B35</f>
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="9">
+        <v>20000</v>
+      </c>
+      <c r="C36" s="38">
+        <v>3</v>
+      </c>
+      <c r="D36" s="9">
+        <v>30000</v>
+      </c>
+      <c r="E36" s="1">
+        <v>2</v>
+      </c>
+      <c r="F36" s="23">
+        <v>10000</v>
+      </c>
+      <c r="G36" s="23"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+      <c r="T36" s="19">
+        <f>B36+C36*D36*0.4+E36*F36</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="17">
-        <v>80000</v>
-      </c>
-      <c r="T36" s="31">
-        <f>B36</f>
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B38" s="9">
+        <v>18000</v>
+      </c>
+      <c r="C38" s="9">
+        <v>2500</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3</v>
+      </c>
+      <c r="E38" s="9">
+        <v>23000</v>
+      </c>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28"/>
+      <c r="T38" s="19">
+        <f>B38+C38+D38*E38*0.4</f>
+        <v>48100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="17">
-        <v>60000</v>
-      </c>
-      <c r="T37" s="31">
-        <f>B37</f>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B40" s="9">
+        <v>150</v>
+      </c>
+      <c r="C40" s="38">
+        <v>160</v>
+      </c>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="T40" s="19">
+        <f>B40*C40</f>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="T38" s="31">
-        <f>SUM(T34:T37)</f>
-        <v>460000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="S39" s="3" t="s">
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T42" s="19">
+        <f>SUM(T34:T40)</f>
+        <v>468100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="49">
+        <v>1</v>
+      </c>
+      <c r="C45" s="50">
+        <v>0.05</v>
+      </c>
+      <c r="D45" s="22">
+        <f>T14</f>
+        <v>87700</v>
+      </c>
+      <c r="E45" s="9">
+        <f>D45*C45</f>
+        <v>4385</v>
+      </c>
+      <c r="T45" s="19">
+        <f>T14*C45</f>
+        <v>4385</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="49">
+        <v>2</v>
+      </c>
+      <c r="C46" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="D46" s="22">
+        <f>T29</f>
+        <v>933080</v>
+      </c>
+      <c r="E46" s="9">
+        <f t="shared" ref="E46:E47" si="3">D46*C46</f>
+        <v>93308</v>
+      </c>
+      <c r="T46" s="19">
+        <f>T29*C46</f>
+        <v>93308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="49">
+        <v>3</v>
+      </c>
+      <c r="C47" s="50">
+        <v>0.15</v>
+      </c>
+      <c r="D47" s="22">
+        <f>T42</f>
+        <v>468100</v>
+      </c>
+      <c r="E47" s="9">
+        <f t="shared" si="3"/>
+        <v>70215</v>
+      </c>
+      <c r="T47" s="19">
+        <f>T42*C47</f>
+        <v>70215</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T48" s="19">
+        <f>SUM(T45:T47)</f>
+        <v>167908</v>
+      </c>
+    </row>
+    <row r="50" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="S50" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="T39" s="34">
-        <f>T38+T29+T14</f>
-        <v>1480780</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="S40" s="3"/>
-      <c r="T40" s="34"/>
+      <c r="T50" s="23">
+        <f>T42+T29+T14+T48</f>
+        <v>1656788</v>
+      </c>
+    </row>
+    <row r="51" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="S51" s="27"/>
+      <c r="T51" s="23"/>
+    </row>
+    <row r="52" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E52" s="52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E53" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="F53" s="54">
+        <f>T14</f>
+        <v>87700</v>
+      </c>
+      <c r="G53" s="54"/>
+    </row>
+    <row r="54" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E54" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="F54" s="55">
+        <f>T29</f>
+        <v>933080</v>
+      </c>
+      <c r="G54" s="55"/>
+    </row>
+    <row r="55" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E55" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" s="54">
+        <f>T42</f>
+        <v>468100</v>
+      </c>
+      <c r="G55" s="54"/>
+    </row>
+    <row r="56" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E56" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" s="54">
+        <f>T48</f>
+        <v>167908</v>
+      </c>
+      <c r="G56" s="56"/>
+    </row>
+    <row r="57" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E57" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="62">
+        <f>SUM(F53:G56)</f>
+        <v>1656788</v>
+      </c>
+      <c r="G57" s="63"/>
+    </row>
+    <row r="58" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E58" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="F58" s="58">
+        <f>F57*0.12</f>
+        <v>198814.56</v>
+      </c>
+      <c r="G58" s="59"/>
+    </row>
+    <row r="59" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E59" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="F59" s="23">
+        <f>F58+F57</f>
+        <v>1855602.56</v>
+      </c>
+      <c r="G59" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="S39:S40"/>
-    <mergeCell ref="T39:T40"/>
+  <mergeCells count="60">
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H38:R38"/>
+    <mergeCell ref="H40:R40"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H34:R34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:R36"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="F19:Q19"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="S50:S51"/>
+    <mergeCell ref="T50:T51"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
@@ -1700,32 +2235,16 @@
     <mergeCell ref="E17:Q17"/>
     <mergeCell ref="E18:Q18"/>
     <mergeCell ref="E3:Q3"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:Q1"/>
     <mergeCell ref="E4:Q4"/>
     <mergeCell ref="E5:Q5"/>
     <mergeCell ref="E6:Q6"/>
     <mergeCell ref="E7:Q7"/>
     <mergeCell ref="E8:Q8"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="F19:Q19"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="L27:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizado el punto estimacion de costes.
Comenzado el punto del presupuesto.
Configuración del excel, añadida financiación.
</commit_message>
<xml_diff>
--- a/Documentos_generados/5. Costes y Justificación técnica/Estimacion costes.xlsx
+++ b/Documentos_generados/5. Costes y Justificación técnica/Estimacion costes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="118">
   <si>
     <t>Estimación costes</t>
   </si>
@@ -216,9 +216,6 @@
     <t>horas / dia</t>
   </si>
   <si>
-    <t>Se pacta este precio con la empresa desarrolladora de SW acorde a los datos de trabajadores</t>
-  </si>
-  <si>
     <t>Almacen</t>
   </si>
   <si>
@@ -301,6 +298,78 @@
   </si>
   <si>
     <t>Medidores de saturación oxigeno en sangre. Capacidad de sincronización Bluetooth con el SW</t>
+  </si>
+  <si>
+    <t>TOTAL CONTINGENCIAS</t>
+  </si>
+  <si>
+    <t>ENERO</t>
+  </si>
+  <si>
+    <t>SEPTIEMBRE</t>
+  </si>
+  <si>
+    <t>OCTUBRE</t>
+  </si>
+  <si>
+    <t>NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>DICIEMBRE</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
+    <t>MARZO</t>
+  </si>
+  <si>
+    <t>ABRIL</t>
+  </si>
+  <si>
+    <t>MAYO</t>
+  </si>
+  <si>
+    <t>JUNIO</t>
+  </si>
+  <si>
+    <t>JULIO</t>
+  </si>
+  <si>
+    <t>AGOSTO</t>
+  </si>
+  <si>
+    <t>COSTES</t>
+  </si>
+  <si>
+    <t>INGRESOS</t>
+  </si>
+  <si>
+    <t>MATERIAL OFICINA</t>
+  </si>
+  <si>
+    <t>MATERIAL TÉCNICO</t>
+  </si>
+  <si>
+    <t>SUBCON. SW</t>
+  </si>
+  <si>
+    <t>SUBCON. ALMACÉN</t>
+  </si>
+  <si>
+    <t>SUBCON. CALLCEN</t>
+  </si>
+  <si>
+    <t>COMPROBACION</t>
+  </si>
+  <si>
+    <t>SUBCON. DATACEN</t>
+  </si>
+  <si>
+    <t>GASTOS POR MES</t>
+  </si>
+  <si>
+    <t>GASTOS ACUMULADOS</t>
   </si>
 </sst>
 </file>
@@ -310,7 +379,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,8 +434,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +553,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -482,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -565,85 +667,121 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,6 +795,290 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ingresos</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$X$2:$AJ$2</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>SEPTIEMBRE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OCTUBRE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NOVIEMBRE</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DICIEMBRE</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ENERO</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FEBRERO</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MARZO</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ABRIL</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MAYO</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>JULIO</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>AGOSTO</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SEPTIEMBRE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$X$12:$AJ$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>444413.87199999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>444413.87199999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>444413.87199999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>888827.74399999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>888827.74399999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>888827.74399999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1111034.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1333241.6159999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1333241.6159999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1777655.4879999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1777655.4879999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1999862.4239999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2222069.36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Costes sin contingencias</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$X$11:$AJ$11</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>75352.307692307688</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230704.61538461538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>386056.92307692306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>541409.23076923075</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>696761.5384615385</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>807759.6794871795</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>934791.15384615387</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1090697.6282051282</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1221270.7692307692</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1335810.576923077</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1488850.3846153847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1641890.1923076925</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1794930.0000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="154199552"/>
+        <c:axId val="141065536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="154199552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141065536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141065536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00\ &quot;€&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154199552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1255059</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>40341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>739588</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -946,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T59"/>
+  <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="S10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z39" sqref="Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,76 +1393,134 @@
     <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.7109375" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
     <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.7109375" style="14" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="36" width="13.28515625" style="38" customWidth="1"/>
+    <col min="38" max="38" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="13" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:38" s="13" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="64"/>
+      <c r="D1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60" t="s">
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="63" t="s">
+      <c r="T1" s="42" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+    </row>
+    <row r="2" spans="1:38" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z2" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA2" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB2" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC2" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD2" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE2" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF2" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG2" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH2" s="73" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI2" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ2" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL2" s="69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="49">
         <v>2000</v>
       </c>
-      <c r="C3" s="37"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
       <c r="R3">
         <v>12</v>
       </c>
@@ -1051,60 +1531,182 @@
         <f>B3*R3</f>
         <v>24000</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V3" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="W3" s="71" t="s">
+        <v>78</v>
+      </c>
+      <c r="X3" s="76">
+        <f>($T$31/13)</f>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="Y3" s="76">
+        <f t="shared" ref="Y3:AJ3" si="0">($T$31/13)</f>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="Z3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AA3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AB3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AC3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AD3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AE3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AF3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AG3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AH3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AI3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AJ3" s="76">
+        <f t="shared" si="0"/>
+        <v>71775.38461538461</v>
+      </c>
+      <c r="AL3" s="70">
+        <f>SUM(X3:AJ3)</f>
+        <v>933080</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="49">
         <v>500</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="49"/>
+      <c r="E4" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
       <c r="T4" s="14">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V4" s="75"/>
+      <c r="W4" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="X4" s="76">
+        <f>($T$3/13)+($T$4/13)+($T$5/13)+($T$6/13)+($T$7/13)</f>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="Y4" s="76">
+        <f t="shared" ref="Y4:AJ4" si="1">($T$3/13)+($T$4/13)+($T$5/13)+($T$6/13)+($T$7/13)</f>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="Z4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AA4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AB4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AC4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AD4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AE4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AF4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AG4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AH4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AI4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AJ4" s="76">
+        <f t="shared" si="1"/>
+        <v>3576.9230769230776</v>
+      </c>
+      <c r="AL4" s="70">
+        <f t="shared" ref="AL4:AL9" si="2">SUM(X4:AJ4)</f>
+        <v>46500.000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="49">
         <v>250</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
       <c r="R5">
         <v>20</v>
       </c>
@@ -1115,33 +1717,86 @@
         <f>B5*R5</f>
         <v>5000</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V5" s="75"/>
+      <c r="W5" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="X5" s="76">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="76">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="76">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="76">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="76">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="76">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="76">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="76">
+        <f>SUM($T$9:$T$13)*0.3/3</f>
+        <v>28875</v>
+      </c>
+      <c r="AF5" s="76">
+        <f t="shared" ref="AF5:AG5" si="3">SUM($T$9:$T$13)*0.3/3</f>
+        <v>28875</v>
+      </c>
+      <c r="AG5" s="76">
+        <f t="shared" si="3"/>
+        <v>28875</v>
+      </c>
+      <c r="AH5" s="76">
+        <f>SUM($T$9:$T$13)*0.7/3</f>
+        <v>67375</v>
+      </c>
+      <c r="AI5" s="76">
+        <f t="shared" ref="AI5:AJ5" si="4">SUM($T$9:$T$13)*0.7/3</f>
+        <v>67375</v>
+      </c>
+      <c r="AJ5" s="76">
+        <f t="shared" si="4"/>
+        <v>67375</v>
+      </c>
+      <c r="AL5" s="70">
+        <f t="shared" si="2"/>
+        <v>288750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="49">
         <v>700</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
       <c r="R6">
         <v>20</v>
       </c>
@@ -1152,33 +1807,66 @@
         <f>B6*R6</f>
         <v>14000</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V6" s="75"/>
+      <c r="W6" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="76">
+        <f>$T$34/4</f>
+        <v>80000</v>
+      </c>
+      <c r="Z6" s="76">
+        <f t="shared" ref="Z6:AB6" si="5">$T$34/4</f>
+        <v>80000</v>
+      </c>
+      <c r="AA6" s="76">
+        <f t="shared" si="5"/>
+        <v>80000</v>
+      </c>
+      <c r="AB6" s="76">
+        <f t="shared" si="5"/>
+        <v>80000</v>
+      </c>
+      <c r="AC6" s="76"/>
+      <c r="AD6" s="76"/>
+      <c r="AE6" s="76"/>
+      <c r="AF6" s="76"/>
+      <c r="AG6" s="76"/>
+      <c r="AH6" s="76"/>
+      <c r="AI6" s="76"/>
+      <c r="AJ6" s="76"/>
+      <c r="AL6" s="70">
+        <f t="shared" si="2"/>
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="49">
         <v>150</v>
       </c>
-      <c r="C7" s="37"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
       <c r="R7">
         <v>20</v>
       </c>
@@ -1189,53 +1877,113 @@
         <f>B7*R7</f>
         <v>3000</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V7" s="75"/>
+      <c r="W7" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="X7" s="76"/>
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="76"/>
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="76"/>
+      <c r="AC7" s="76">
+        <f>$T$36/3</f>
+        <v>25333.333333333332</v>
+      </c>
+      <c r="AD7" s="76">
+        <f t="shared" ref="AD7:AE7" si="6">$T$36/3</f>
+        <v>25333.333333333332</v>
+      </c>
+      <c r="AE7" s="76">
+        <f t="shared" si="6"/>
+        <v>25333.333333333332</v>
+      </c>
+      <c r="AF7" s="76"/>
+      <c r="AG7" s="76"/>
+      <c r="AH7" s="76"/>
+      <c r="AI7" s="76"/>
+      <c r="AJ7" s="76"/>
+      <c r="AL7" s="70">
+        <f t="shared" si="2"/>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="V8" s="75"/>
+      <c r="W8" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="X8" s="76"/>
+      <c r="Y8" s="76"/>
+      <c r="Z8" s="76"/>
+      <c r="AA8" s="76"/>
+      <c r="AB8" s="76"/>
+      <c r="AC8" s="76"/>
+      <c r="AD8" s="76">
+        <f>$T$38/3</f>
+        <v>16033.333333333334</v>
+      </c>
+      <c r="AE8" s="76">
+        <f t="shared" ref="AE8:AF8" si="7">$T$38/3</f>
+        <v>16033.333333333334</v>
+      </c>
+      <c r="AF8" s="76">
+        <f t="shared" si="7"/>
+        <v>16033.333333333334</v>
+      </c>
+      <c r="AG8" s="76"/>
+      <c r="AH8" s="76"/>
+      <c r="AI8" s="76"/>
+      <c r="AJ8" s="76"/>
+      <c r="AL8" s="70">
+        <f t="shared" si="2"/>
+        <v>48100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="49">
         <v>60</v>
       </c>
-      <c r="C9" s="37"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="50"/>
       <c r="R9">
         <v>550</v>
       </c>
@@ -1246,33 +1994,78 @@
         <f>B9*R9</f>
         <v>33000</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V9" s="75"/>
+      <c r="W9" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="X9" s="76"/>
+      <c r="Y9" s="76"/>
+      <c r="Z9" s="76"/>
+      <c r="AA9" s="76"/>
+      <c r="AB9" s="76"/>
+      <c r="AC9" s="76">
+        <f>$T$40/8</f>
+        <v>10312.5</v>
+      </c>
+      <c r="AD9" s="76">
+        <f t="shared" ref="AD9:AJ9" si="8">$T$40/8</f>
+        <v>10312.5</v>
+      </c>
+      <c r="AE9" s="76">
+        <f t="shared" si="8"/>
+        <v>10312.5</v>
+      </c>
+      <c r="AF9" s="76">
+        <f t="shared" si="8"/>
+        <v>10312.5</v>
+      </c>
+      <c r="AG9" s="76">
+        <f t="shared" si="8"/>
+        <v>10312.5</v>
+      </c>
+      <c r="AH9" s="76">
+        <f t="shared" si="8"/>
+        <v>10312.5</v>
+      </c>
+      <c r="AI9" s="76">
+        <f t="shared" si="8"/>
+        <v>10312.5</v>
+      </c>
+      <c r="AJ9" s="76">
+        <f t="shared" si="8"/>
+        <v>10312.5</v>
+      </c>
+      <c r="AL9" s="70">
+        <f t="shared" si="2"/>
+        <v>82500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="49">
         <v>35</v>
       </c>
-      <c r="C10" s="37"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
       <c r="R10">
         <v>550</v>
       </c>
@@ -1280,36 +2073,92 @@
         <v>17</v>
       </c>
       <c r="T10" s="14">
-        <f t="shared" ref="T10:T13" si="0">B10*R10</f>
+        <f t="shared" ref="T10:T13" si="9">B10*R10</f>
         <v>19250</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V10" s="71"/>
+      <c r="W10" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="X10" s="76">
+        <f>SUM(X3:X9)</f>
+        <v>75352.307692307688</v>
+      </c>
+      <c r="Y10" s="76">
+        <f t="shared" ref="Y10:AJ10" si="10">SUM(Y3:Y9)</f>
+        <v>155352.30769230769</v>
+      </c>
+      <c r="Z10" s="76">
+        <f t="shared" si="10"/>
+        <v>155352.30769230769</v>
+      </c>
+      <c r="AA10" s="76">
+        <f t="shared" si="10"/>
+        <v>155352.30769230769</v>
+      </c>
+      <c r="AB10" s="76">
+        <f t="shared" si="10"/>
+        <v>155352.30769230769</v>
+      </c>
+      <c r="AC10" s="76">
+        <f t="shared" si="10"/>
+        <v>110998.14102564102</v>
+      </c>
+      <c r="AD10" s="76">
+        <f t="shared" si="10"/>
+        <v>127031.47435897434</v>
+      </c>
+      <c r="AE10" s="76">
+        <f t="shared" si="10"/>
+        <v>155906.47435897434</v>
+      </c>
+      <c r="AF10" s="76">
+        <f t="shared" si="10"/>
+        <v>130573.14102564102</v>
+      </c>
+      <c r="AG10" s="76">
+        <f t="shared" si="10"/>
+        <v>114539.80769230769</v>
+      </c>
+      <c r="AH10" s="76">
+        <f t="shared" si="10"/>
+        <v>153039.80769230769</v>
+      </c>
+      <c r="AI10" s="76">
+        <f t="shared" si="10"/>
+        <v>153039.80769230769</v>
+      </c>
+      <c r="AJ10" s="76">
+        <f t="shared" si="10"/>
+        <v>153039.80769230769</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="37">
+        <v>92</v>
+      </c>
+      <c r="B11" s="49">
         <v>200</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
+      <c r="E11" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
       <c r="R11">
         <v>550</v>
       </c>
@@ -1317,36 +2166,92 @@
         <v>17</v>
       </c>
       <c r="T11" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>110000</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V11" s="71"/>
+      <c r="W11" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="X11" s="76">
+        <f>X10</f>
+        <v>75352.307692307688</v>
+      </c>
+      <c r="Y11" s="76">
+        <f>X10+Y10</f>
+        <v>230704.61538461538</v>
+      </c>
+      <c r="Z11" s="76">
+        <f>Y11+Z10</f>
+        <v>386056.92307692306</v>
+      </c>
+      <c r="AA11" s="76">
+        <f t="shared" ref="AA11:AJ11" si="11">Z11+AA10</f>
+        <v>541409.23076923075</v>
+      </c>
+      <c r="AB11" s="76">
+        <f t="shared" si="11"/>
+        <v>696761.5384615385</v>
+      </c>
+      <c r="AC11" s="76">
+        <f t="shared" si="11"/>
+        <v>807759.6794871795</v>
+      </c>
+      <c r="AD11" s="76">
+        <f t="shared" si="11"/>
+        <v>934791.15384615387</v>
+      </c>
+      <c r="AE11" s="76">
+        <f t="shared" si="11"/>
+        <v>1090697.6282051282</v>
+      </c>
+      <c r="AF11" s="76">
+        <f t="shared" si="11"/>
+        <v>1221270.7692307692</v>
+      </c>
+      <c r="AG11" s="76">
+        <f t="shared" si="11"/>
+        <v>1335810.576923077</v>
+      </c>
+      <c r="AH11" s="76">
+        <f t="shared" si="11"/>
+        <v>1488850.3846153847</v>
+      </c>
+      <c r="AI11" s="76">
+        <f t="shared" si="11"/>
+        <v>1641890.1923076925</v>
+      </c>
+      <c r="AJ11" s="76">
+        <f t="shared" si="11"/>
+        <v>1794930.0000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="37">
+        <v>91</v>
+      </c>
+      <c r="B12" s="49">
         <v>80</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
       <c r="R12">
         <v>550</v>
       </c>
@@ -1354,36 +2259,92 @@
         <v>17</v>
       </c>
       <c r="T12" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>44000</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V12" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="W12" s="72"/>
+      <c r="X12" s="77">
+        <f>$B$59*0.2</f>
+        <v>444413.87199999997</v>
+      </c>
+      <c r="Y12" s="77">
+        <f t="shared" ref="Y12:AA12" si="12">$B$59*0.2</f>
+        <v>444413.87199999997</v>
+      </c>
+      <c r="Z12" s="77">
+        <f t="shared" si="12"/>
+        <v>444413.87199999997</v>
+      </c>
+      <c r="AA12" s="77">
+        <f>$B$59*0.4</f>
+        <v>888827.74399999995</v>
+      </c>
+      <c r="AB12" s="77">
+        <f t="shared" ref="AB12:AF12" si="13">$B$59*0.4</f>
+        <v>888827.74399999995</v>
+      </c>
+      <c r="AC12" s="77">
+        <f t="shared" si="13"/>
+        <v>888827.74399999995</v>
+      </c>
+      <c r="AD12" s="77">
+        <f>$B$59*0.5</f>
+        <v>1111034.68</v>
+      </c>
+      <c r="AE12" s="77">
+        <f>$B$59*0.6</f>
+        <v>1333241.6159999999</v>
+      </c>
+      <c r="AF12" s="77">
+        <f>$B$59*0.6</f>
+        <v>1333241.6159999999</v>
+      </c>
+      <c r="AG12" s="77">
+        <f>$B$59*0.8</f>
+        <v>1777655.4879999999</v>
+      </c>
+      <c r="AH12" s="77">
+        <f>$B$59*0.8</f>
+        <v>1777655.4879999999</v>
+      </c>
+      <c r="AI12" s="77">
+        <f>$B$59*0.9</f>
+        <v>1999862.4239999999</v>
+      </c>
+      <c r="AJ12" s="77">
+        <f>$B$59</f>
+        <v>2222069.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="63">
         <v>150</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="63"/>
       <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
       <c r="R13">
         <v>550</v>
       </c>
@@ -1391,25 +2352,38 @@
         <v>17</v>
       </c>
       <c r="T13" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>82500</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="38"/>
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="38"/>
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="38"/>
+      <c r="AG13" s="38"/>
+      <c r="AH13" s="38"/>
+      <c r="AI13" s="38"/>
+      <c r="AJ13" s="38"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="T14" s="59">
+      <c r="T14" s="40">
         <f>SUM(T1:T13)</f>
         <v>335250</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+    <row r="15" spans="1:38" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>5</v>
       </c>
@@ -1425,19 +2399,19 @@
         <f>B17/1764</f>
         <v>51.020408163265309</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
       <c r="R17">
         <v>1</v>
       </c>
@@ -1460,19 +2434,19 @@
         <f>B18/1764</f>
         <v>39.682539682539684</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
       <c r="R18">
         <v>4</v>
       </c>
@@ -1485,42 +2459,42 @@
       </c>
     </row>
     <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
     </row>
     <row r="20" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46" t="s">
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="47" t="s">
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="48" t="s">
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
     </row>
     <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F21" s="4" t="s">
@@ -1561,17 +2535,17 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="54">
         <v>56000</v>
       </c>
-      <c r="C22" s="44">
+      <c r="C22" s="56">
         <f>B22/1764</f>
         <v>31.746031746031747</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="55" t="s">
         <v>49</v>
       </c>
       <c r="E22" t="s">
@@ -1619,10 +2593,10 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="40"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="55"/>
       <c r="E23" t="s">
         <v>26</v>
       </c>
@@ -1668,10 +2642,10 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="40"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="55"/>
       <c r="E24" t="s">
         <v>27</v>
       </c>
@@ -1717,17 +2691,17 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="49">
+      <c r="B25" s="54">
         <v>44750</v>
       </c>
-      <c r="C25" s="44">
-        <f t="shared" ref="C25" si="1">B25/1764</f>
+      <c r="C25" s="56">
+        <f t="shared" ref="C25" si="14">B25/1764</f>
         <v>25.368480725623584</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="55" t="s">
         <v>49</v>
       </c>
       <c r="E25" t="s">
@@ -1755,10 +2729,10 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="40"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="55"/>
       <c r="E26" t="s">
         <v>29</v>
       </c>
@@ -1774,39 +2748,39 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="40"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="43" t="s">
+      <c r="F27" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="43"/>
+      <c r="G27" s="59"/>
       <c r="H27">
         <f>SUM(H22:H26)</f>
         <v>150845</v>
       </c>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="43"/>
+      <c r="J27" s="59"/>
       <c r="K27">
         <f>SUM(K22:K26)</f>
         <v>114175</v>
       </c>
-      <c r="L27" s="43" t="s">
+      <c r="L27" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="M27" s="43"/>
+      <c r="M27" s="59"/>
       <c r="N27">
         <f>SUM(N22:N26)</f>
         <v>109700</v>
       </c>
-      <c r="O27" s="43" t="s">
+      <c r="O27" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="P27" s="43"/>
+      <c r="P27" s="59"/>
       <c r="Q27">
         <f>SUM(Q22:Q26)</f>
         <v>188360</v>
@@ -1817,31 +2791,31 @@
       </c>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="49">
+      <c r="B28" s="54">
         <v>31200</v>
       </c>
-      <c r="C28" s="44">
-        <f t="shared" ref="C28" si="2">B28/1764</f>
+      <c r="C28" s="56">
+        <f t="shared" ref="C28" si="15">B28/1764</f>
         <v>17.687074829931973</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="55" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="40"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="55"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="40"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="55"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
@@ -1850,7 +2824,7 @@
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="2"/>
-      <c r="T31" s="59">
+      <c r="T31" s="40">
         <f>SUM(T15:T28)</f>
         <v>933080</v>
       </c>
@@ -1862,7 +2836,7 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="58" t="s">
+      <c r="A33" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="20" t="s">
@@ -1900,19 +2874,17 @@
       <c r="F34">
         <v>20</v>
       </c>
-      <c r="H34" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="39"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="50"/>
+      <c r="P34" s="50"/>
+      <c r="Q34" s="50"/>
+      <c r="R34" s="50"/>
       <c r="T34" s="14">
         <f>B34*C34*D34*E34*F34</f>
         <v>320000</v>
@@ -1920,21 +2892,21 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B35" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="E35" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="21" t="s">
+      <c r="F35" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="50" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" s="50"/>
+      <c r="G35" s="52"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
@@ -1952,21 +2924,21 @@
       <c r="E36" s="1">
         <v>2</v>
       </c>
-      <c r="F36" s="37">
+      <c r="F36" s="49">
         <v>10000</v>
       </c>
-      <c r="G36" s="37"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="39"/>
-      <c r="R36" s="39"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
       <c r="T36" s="14">
         <f>B36+C36*D36*0.4+E36*F36</f>
         <v>76000</v>
@@ -1974,16 +2946,16 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B37" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="24" t="s">
         <v>72</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>73</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>61</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -2003,17 +2975,17 @@
       <c r="E38" s="9">
         <v>23000</v>
       </c>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="39"/>
-      <c r="R38" s="39"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
       <c r="T38" s="14">
         <f>B38+C38+D38*E38*0.4</f>
         <v>48100</v>
@@ -2021,10 +2993,10 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B39" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="27" t="s">
         <v>75</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -2037,17 +3009,17 @@
       <c r="C40" s="18">
         <v>550</v>
       </c>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="39"/>
-      <c r="N40" s="39"/>
-      <c r="O40" s="39"/>
-      <c r="P40" s="39"/>
-      <c r="Q40" s="39"/>
-      <c r="R40" s="39"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="50"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="50"/>
+      <c r="R40" s="50"/>
       <c r="T40" s="14">
         <f>B40*C40</f>
         <v>82500</v>
@@ -2057,30 +3029,28 @@
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T42" s="59">
+      <c r="T41" s="40">
         <f>SUM(T34:T40)</f>
         <v>526600</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="58" t="s">
-        <v>77</v>
+      <c r="A44" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="B44" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="D44" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="28">
         <v>1</v>
@@ -2103,7 +3073,7 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" s="28">
         <v>2</v>
@@ -2116,7 +3086,7 @@
         <v>933080</v>
       </c>
       <c r="E46" s="9">
-        <f t="shared" ref="E46:E47" si="3">D46*C46</f>
+        <f t="shared" ref="E46:E47" si="16">D46*C46</f>
         <v>93308</v>
       </c>
       <c r="T46" s="14">
@@ -2126,7 +3096,7 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" s="28">
         <v>3</v>
@@ -2135,148 +3105,136 @@
         <v>0.15</v>
       </c>
       <c r="D47" s="17">
-        <f>T42</f>
+        <f>T41</f>
         <v>526600</v>
       </c>
       <c r="E47" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>78990</v>
       </c>
       <c r="T47" s="14">
-        <f>T42*C47</f>
+        <f>T41*C47</f>
         <v>78990</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="T48" s="59">
+      <c r="A48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T48" s="40">
         <f>SUM(T45:T47)</f>
         <v>189060.5</v>
       </c>
     </row>
-    <row r="50" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="S50" s="40" t="s">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S50" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="T50" s="37">
-        <f>T42+T31+T14+T48</f>
+      <c r="T50" s="67">
+        <f>T41+T31+T14+T48</f>
         <v>1983990.5</v>
       </c>
     </row>
-    <row r="51" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="S51" s="40"/>
-      <c r="T51" s="37"/>
-    </row>
-    <row r="52" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E52" s="31" t="s">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S51" s="66"/>
+      <c r="T51" s="67"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52"/>
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="53" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E53" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="51">
+      <c r="B53" s="43">
         <f>T14</f>
         <v>335250</v>
       </c>
-      <c r="G53" s="51"/>
-    </row>
-    <row r="54" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E54" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F54" s="57">
+      <c r="C53" s="43"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="51">
         <f>T31</f>
         <v>933080</v>
       </c>
-      <c r="G54" s="57"/>
-    </row>
-    <row r="55" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E55" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="F55" s="51">
-        <f>T42</f>
+      <c r="C54" s="51"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="43">
+        <f>T41</f>
         <v>526600</v>
       </c>
-      <c r="G55" s="51"/>
-    </row>
-    <row r="56" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E56" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="51">
+      <c r="C55" s="43"/>
+      <c r="D55" s="37">
+        <f>SUM(B53:C55)</f>
+        <v>1794930</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="43">
         <f>T48</f>
         <v>189060.5</v>
       </c>
-      <c r="G56" s="52"/>
-    </row>
-    <row r="57" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E57" s="35" t="s">
+      <c r="C56" s="44"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="45">
+        <f>SUM(B53:C56)</f>
+        <v>1983990.5</v>
+      </c>
+      <c r="C57" s="46"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="F57" s="53">
-        <f>SUM(F53:G56)</f>
-        <v>1983990.5</v>
-      </c>
-      <c r="G57" s="54"/>
-    </row>
-    <row r="58" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E58" s="33" t="s">
+      <c r="B58" s="47">
+        <f>B57*0.12</f>
+        <v>238078.86</v>
+      </c>
+      <c r="C58" s="48"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="F58" s="55">
-        <f>F57*0.12</f>
-        <v>238078.86</v>
-      </c>
-      <c r="G58" s="56"/>
-    </row>
-    <row r="59" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E59" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="F59" s="37">
-        <f>F58+F57</f>
+      <c r="B59" s="49">
+        <f>B58+B57</f>
         <v>2222069.36</v>
       </c>
-      <c r="G59" s="39"/>
+      <c r="C59" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H38:R38"/>
-    <mergeCell ref="H40:R40"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H34:R34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:R36"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="F19:Q19"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
+  <mergeCells count="63">
+    <mergeCell ref="V3:V9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="E4:Q4"/>
+    <mergeCell ref="E5:Q5"/>
+    <mergeCell ref="E6:Q6"/>
+    <mergeCell ref="E7:Q7"/>
+    <mergeCell ref="E8:Q8"/>
+    <mergeCell ref="E11:Q11"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="S50:S51"/>
     <mergeCell ref="T50:T51"/>
     <mergeCell ref="B3:C3"/>
@@ -2293,21 +3251,44 @@
     <mergeCell ref="E17:Q17"/>
     <mergeCell ref="E18:Q18"/>
     <mergeCell ref="E3:Q3"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="E5:Q5"/>
-    <mergeCell ref="E6:Q6"/>
-    <mergeCell ref="E7:Q7"/>
-    <mergeCell ref="E8:Q8"/>
-    <mergeCell ref="E11:Q11"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="F19:Q19"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="H34:R34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:R36"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="H38:R38"/>
+    <mergeCell ref="H40:R40"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>